<commit_message>
ESP12 dev board PCB update
</commit_message>
<xml_diff>
--- a/_PCB/ESP12_DevBoard/OUTPUT/BOM.xlsx
+++ b/_PCB/ESP12_DevBoard/OUTPUT/BOM.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\angrypig\Angrypig\Dev\hardware\_PCB\ESP12_DevBoard\OUTPUT\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1046EDAC-8631-487A-90F7-A6780CEAB8B1}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0EC105C9-A91B-4DFA-BF73-CCFA67C826D0}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5760" yWindow="3396" windowWidth="17280" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2808" yWindow="2880" windowWidth="17280" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="BOM_CSV" sheetId="1" r:id="rId1"/>
@@ -1038,63 +1038,63 @@
     <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="20" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1">
-      <alignment vertical="center"/>
-    </xf>
   </cellXfs>
   <cellStyles count="43">
-    <cellStyle name="20% - 강조색1" xfId="19" builtinId="30" customBuiltin="1"/>
-    <cellStyle name="20% - 강조색2" xfId="23" builtinId="34" customBuiltin="1"/>
-    <cellStyle name="20% - 강조색3" xfId="27" builtinId="38" customBuiltin="1"/>
-    <cellStyle name="20% - 강조색4" xfId="31" builtinId="42" customBuiltin="1"/>
-    <cellStyle name="20% - 강조색5" xfId="35" builtinId="46" customBuiltin="1"/>
-    <cellStyle name="20% - 강조색6" xfId="39" builtinId="50" customBuiltin="1"/>
-    <cellStyle name="40% - 강조색1" xfId="20" builtinId="31" customBuiltin="1"/>
-    <cellStyle name="40% - 강조색2" xfId="24" builtinId="35" customBuiltin="1"/>
-    <cellStyle name="40% - 강조색3" xfId="28" builtinId="39" customBuiltin="1"/>
-    <cellStyle name="40% - 강조색4" xfId="32" builtinId="43" customBuiltin="1"/>
-    <cellStyle name="40% - 강조색5" xfId="36" builtinId="47" customBuiltin="1"/>
-    <cellStyle name="40% - 강조색6" xfId="40" builtinId="51" customBuiltin="1"/>
-    <cellStyle name="60% - 강조색1" xfId="21" builtinId="32" customBuiltin="1"/>
-    <cellStyle name="60% - 강조색2" xfId="25" builtinId="36" customBuiltin="1"/>
-    <cellStyle name="60% - 강조색3" xfId="29" builtinId="40" customBuiltin="1"/>
-    <cellStyle name="60% - 강조색4" xfId="33" builtinId="44" customBuiltin="1"/>
-    <cellStyle name="60% - 강조색5" xfId="37" builtinId="48" customBuiltin="1"/>
-    <cellStyle name="60% - 강조색6" xfId="41" builtinId="52" customBuiltin="1"/>
-    <cellStyle name="강조색1" xfId="18" builtinId="29" customBuiltin="1"/>
-    <cellStyle name="강조색2" xfId="22" builtinId="33" customBuiltin="1"/>
-    <cellStyle name="강조색3" xfId="26" builtinId="37" customBuiltin="1"/>
-    <cellStyle name="강조색4" xfId="30" builtinId="41" customBuiltin="1"/>
-    <cellStyle name="강조색5" xfId="34" builtinId="45" customBuiltin="1"/>
-    <cellStyle name="강조색6" xfId="38" builtinId="49" customBuiltin="1"/>
-    <cellStyle name="경고문" xfId="14" builtinId="11" customBuiltin="1"/>
-    <cellStyle name="계산" xfId="11" builtinId="22" customBuiltin="1"/>
-    <cellStyle name="나쁨" xfId="7" builtinId="27" customBuiltin="1"/>
-    <cellStyle name="메모" xfId="15" builtinId="10" customBuiltin="1"/>
-    <cellStyle name="보통" xfId="8" builtinId="28" customBuiltin="1"/>
-    <cellStyle name="설명 텍스트" xfId="16" builtinId="53" customBuiltin="1"/>
-    <cellStyle name="셀 확인" xfId="13" builtinId="23" customBuiltin="1"/>
-    <cellStyle name="연결된 셀" xfId="12" builtinId="24" customBuiltin="1"/>
-    <cellStyle name="요약" xfId="17" builtinId="25" customBuiltin="1"/>
-    <cellStyle name="입력" xfId="9" builtinId="20" customBuiltin="1"/>
-    <cellStyle name="제목" xfId="1" builtinId="15" customBuiltin="1"/>
-    <cellStyle name="제목 1" xfId="2" builtinId="16" customBuiltin="1"/>
-    <cellStyle name="제목 2" xfId="3" builtinId="17" customBuiltin="1"/>
-    <cellStyle name="제목 3" xfId="4" builtinId="18" customBuiltin="1"/>
-    <cellStyle name="제목 4" xfId="5" builtinId="19" customBuiltin="1"/>
-    <cellStyle name="좋음" xfId="6" builtinId="26" customBuiltin="1"/>
-    <cellStyle name="출력" xfId="10" builtinId="21" customBuiltin="1"/>
-    <cellStyle name="표준" xfId="0" builtinId="0"/>
-    <cellStyle name="하이퍼링크" xfId="42" builtinId="8"/>
+    <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
+    <cellStyle name="20% - Accent2" xfId="23" builtinId="34" customBuiltin="1"/>
+    <cellStyle name="20% - Accent3" xfId="27" builtinId="38" customBuiltin="1"/>
+    <cellStyle name="20% - Accent4" xfId="31" builtinId="42" customBuiltin="1"/>
+    <cellStyle name="20% - Accent5" xfId="35" builtinId="46" customBuiltin="1"/>
+    <cellStyle name="20% - Accent6" xfId="39" builtinId="50" customBuiltin="1"/>
+    <cellStyle name="40% - Accent1" xfId="20" builtinId="31" customBuiltin="1"/>
+    <cellStyle name="40% - Accent2" xfId="24" builtinId="35" customBuiltin="1"/>
+    <cellStyle name="40% - Accent3" xfId="28" builtinId="39" customBuiltin="1"/>
+    <cellStyle name="40% - Accent4" xfId="32" builtinId="43" customBuiltin="1"/>
+    <cellStyle name="40% - Accent5" xfId="36" builtinId="47" customBuiltin="1"/>
+    <cellStyle name="40% - Accent6" xfId="40" builtinId="51" customBuiltin="1"/>
+    <cellStyle name="60% - Accent1" xfId="21" builtinId="32" customBuiltin="1"/>
+    <cellStyle name="60% - Accent2" xfId="25" builtinId="36" customBuiltin="1"/>
+    <cellStyle name="60% - Accent3" xfId="29" builtinId="40" customBuiltin="1"/>
+    <cellStyle name="60% - Accent4" xfId="33" builtinId="44" customBuiltin="1"/>
+    <cellStyle name="60% - Accent5" xfId="37" builtinId="48" customBuiltin="1"/>
+    <cellStyle name="60% - Accent6" xfId="41" builtinId="52" customBuiltin="1"/>
+    <cellStyle name="Accent1" xfId="18" builtinId="29" customBuiltin="1"/>
+    <cellStyle name="Accent2" xfId="22" builtinId="33" customBuiltin="1"/>
+    <cellStyle name="Accent3" xfId="26" builtinId="37" customBuiltin="1"/>
+    <cellStyle name="Accent4" xfId="30" builtinId="41" customBuiltin="1"/>
+    <cellStyle name="Accent5" xfId="34" builtinId="45" customBuiltin="1"/>
+    <cellStyle name="Accent6" xfId="38" builtinId="49" customBuiltin="1"/>
+    <cellStyle name="Bad" xfId="7" builtinId="27" customBuiltin="1"/>
+    <cellStyle name="Calculation" xfId="11" builtinId="22" customBuiltin="1"/>
+    <cellStyle name="Check Cell" xfId="13" builtinId="23" customBuiltin="1"/>
+    <cellStyle name="Explanatory Text" xfId="16" builtinId="53" customBuiltin="1"/>
+    <cellStyle name="Good" xfId="6" builtinId="26" customBuiltin="1"/>
+    <cellStyle name="Heading 1" xfId="2" builtinId="16" customBuiltin="1"/>
+    <cellStyle name="Heading 2" xfId="3" builtinId="17" customBuiltin="1"/>
+    <cellStyle name="Heading 3" xfId="4" builtinId="18" customBuiltin="1"/>
+    <cellStyle name="Heading 4" xfId="5" builtinId="19" customBuiltin="1"/>
+    <cellStyle name="Hyperlink" xfId="42" builtinId="8"/>
+    <cellStyle name="Input" xfId="9" builtinId="20" customBuiltin="1"/>
+    <cellStyle name="Linked Cell" xfId="12" builtinId="24" customBuiltin="1"/>
+    <cellStyle name="Neutral" xfId="8" builtinId="28" customBuiltin="1"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Note" xfId="15" builtinId="10" customBuiltin="1"/>
+    <cellStyle name="Output" xfId="10" builtinId="21" customBuiltin="1"/>
+    <cellStyle name="Title" xfId="1" builtinId="15" customBuiltin="1"/>
+    <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
+    <cellStyle name="Warning Text" xfId="14" builtinId="11" customBuiltin="1"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1110,7 +1110,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 테마">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -1408,15 +1408,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B2:J29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+    <sheetView tabSelected="1" topLeftCell="F7" workbookViewId="0">
+      <selection activeCell="H29" sqref="H29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
   <cols>
     <col min="1" max="1" width="2.59765625" customWidth="1"/>
     <col min="2" max="2" width="4.296875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="24.19921875" style="9" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="24.19921875" style="8" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="14.59765625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="18.69921875" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="33.59765625" bestFit="1" customWidth="1"/>
@@ -1426,23 +1426,23 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:10" x14ac:dyDescent="0.4">
-      <c r="B2" s="6" t="s">
+      <c r="B2" s="9" t="s">
         <v>84</v>
       </c>
-      <c r="C2" s="6"/>
-      <c r="D2" s="6"/>
-      <c r="E2" s="6"/>
-      <c r="F2" s="6"/>
-      <c r="G2" s="6"/>
-      <c r="H2" s="6"/>
-      <c r="I2" s="6"/>
-      <c r="J2" s="6"/>
+      <c r="C2" s="9"/>
+      <c r="D2" s="9"/>
+      <c r="E2" s="9"/>
+      <c r="F2" s="9"/>
+      <c r="G2" s="9"/>
+      <c r="H2" s="9"/>
+      <c r="I2" s="9"/>
+      <c r="J2" s="9"/>
     </row>
     <row r="3" spans="2:10" x14ac:dyDescent="0.4">
       <c r="B3" s="2" t="s">
         <v>83</v>
       </c>
-      <c r="C3" s="7" t="s">
+      <c r="C3" s="6" t="s">
         <v>0</v>
       </c>
       <c r="D3" s="2" t="s">
@@ -1471,7 +1471,7 @@
       <c r="B4" s="1">
         <v>2</v>
       </c>
-      <c r="C4" s="8" t="s">
+      <c r="C4" s="7" t="s">
         <v>17</v>
       </c>
       <c r="D4" s="1" t="s">
@@ -1487,7 +1487,7 @@
         <v>21</v>
       </c>
       <c r="H4" s="5">
-        <f>(I4*B4)</f>
+        <f t="shared" ref="H4:H26" si="0">(I4*B4)</f>
         <v>2.8000000000000001E-2</v>
       </c>
       <c r="I4" s="5">
@@ -1499,9 +1499,9 @@
     </row>
     <row r="5" spans="2:10" x14ac:dyDescent="0.4">
       <c r="B5" s="1">
-        <v>6</v>
-      </c>
-      <c r="C5" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="C5" s="7" t="s">
         <v>116</v>
       </c>
       <c r="D5" s="1" t="s">
@@ -1517,8 +1517,8 @@
         <v>22</v>
       </c>
       <c r="H5" s="5">
-        <f>(I5*B5)</f>
-        <v>3.6000000000000004E-2</v>
+        <f t="shared" si="0"/>
+        <v>0.03</v>
       </c>
       <c r="I5" s="5">
         <v>6.0000000000000001E-3</v>
@@ -1531,7 +1531,7 @@
       <c r="B6" s="1">
         <v>2</v>
       </c>
-      <c r="C6" s="8" t="s">
+      <c r="C6" s="7" t="s">
         <v>23</v>
       </c>
       <c r="D6" s="1" t="s">
@@ -1547,7 +1547,7 @@
         <v>25</v>
       </c>
       <c r="H6" s="5">
-        <f>(I6*B6)</f>
+        <f t="shared" si="0"/>
         <v>0.19220000000000001</v>
       </c>
       <c r="I6" s="5">
@@ -1561,7 +1561,7 @@
       <c r="B7" s="1">
         <v>2</v>
       </c>
-      <c r="C7" s="8" t="s">
+      <c r="C7" s="7" t="s">
         <v>117</v>
       </c>
       <c r="D7" s="1" t="s">
@@ -1577,7 +1577,7 @@
         <v>33</v>
       </c>
       <c r="H7" s="5">
-        <f>(I7*B7)</f>
+        <f t="shared" si="0"/>
         <v>0.27039999999999997</v>
       </c>
       <c r="I7" s="5">
@@ -1591,7 +1591,7 @@
       <c r="B8" s="1">
         <v>2</v>
       </c>
-      <c r="C8" s="8" t="s">
+      <c r="C8" s="7" t="s">
         <v>34</v>
       </c>
       <c r="D8" s="1" t="s">
@@ -1607,7 +1607,7 @@
         <v>38</v>
       </c>
       <c r="H8" s="5">
-        <f>(I8*B8)</f>
+        <f t="shared" si="0"/>
         <v>5.2999999999999999E-2</v>
       </c>
       <c r="I8" s="5">
@@ -1621,7 +1621,7 @@
       <c r="B9" s="1">
         <v>2</v>
       </c>
-      <c r="C9" s="8" t="s">
+      <c r="C9" s="7" t="s">
         <v>71</v>
       </c>
       <c r="D9" s="1" t="s">
@@ -1637,7 +1637,7 @@
         <v>72</v>
       </c>
       <c r="H9" s="5">
-        <f>(I9*B9)</f>
+        <f t="shared" si="0"/>
         <v>2.3199999999999998E-2</v>
       </c>
       <c r="I9" s="5">
@@ -1651,7 +1651,7 @@
       <c r="B10" s="1">
         <v>1</v>
       </c>
-      <c r="C10" s="8" t="s">
+      <c r="C10" s="7" t="s">
         <v>79</v>
       </c>
       <c r="D10" s="1" t="s">
@@ -1667,7 +1667,7 @@
         <v>80</v>
       </c>
       <c r="H10" s="5">
-        <f>(I10*B10)</f>
+        <f t="shared" si="0"/>
         <v>0.43109999999999998</v>
       </c>
       <c r="I10" s="5">
@@ -1681,7 +1681,7 @@
       <c r="B11" s="1">
         <v>5</v>
       </c>
-      <c r="C11" s="8" t="s">
+      <c r="C11" s="7" t="s">
         <v>7</v>
       </c>
       <c r="D11" s="1">
@@ -1695,7 +1695,7 @@
         <v>99990988</v>
       </c>
       <c r="H11" s="5">
-        <f>(I11*B11)</f>
+        <f t="shared" si="0"/>
         <v>0.19900000000000001</v>
       </c>
       <c r="I11" s="5">
@@ -1709,7 +1709,7 @@
       <c r="B12" s="1">
         <v>1</v>
       </c>
-      <c r="C12" s="8" t="s">
+      <c r="C12" s="7" t="s">
         <v>8</v>
       </c>
       <c r="D12" s="1">
@@ -1723,7 +1723,7 @@
         <v>99990992</v>
       </c>
       <c r="H12" s="5">
-        <f>(I12*B12)</f>
+        <f t="shared" si="0"/>
         <v>0.51700000000000002</v>
       </c>
       <c r="I12" s="5">
@@ -1737,7 +1737,7 @@
       <c r="B13" s="1">
         <v>1</v>
       </c>
-      <c r="C13" s="8" t="s">
+      <c r="C13" s="7" t="s">
         <v>4</v>
       </c>
       <c r="D13" s="1">
@@ -1751,7 +1751,7 @@
         <v>22035025</v>
       </c>
       <c r="H13" s="5">
-        <f>(I13*B13)</f>
+        <f t="shared" si="0"/>
         <v>3.27E-2</v>
       </c>
       <c r="I13" s="5">
@@ -1765,7 +1765,7 @@
       <c r="B14" s="1">
         <v>3</v>
       </c>
-      <c r="C14" s="8" t="s">
+      <c r="C14" s="7" t="s">
         <v>6</v>
       </c>
       <c r="D14" s="1">
@@ -1779,7 +1779,7 @@
         <v>22035035</v>
       </c>
       <c r="H14" s="5">
-        <f>(I14*B14)</f>
+        <f t="shared" si="0"/>
         <v>9.7500000000000003E-2</v>
       </c>
       <c r="I14" s="5">
@@ -1793,7 +1793,7 @@
       <c r="B15" s="1">
         <v>1</v>
       </c>
-      <c r="C15" s="8" t="s">
+      <c r="C15" s="7" t="s">
         <v>52</v>
       </c>
       <c r="D15" s="1" t="s">
@@ -1809,7 +1809,7 @@
         <v>56</v>
       </c>
       <c r="H15" s="5">
-        <f>(I15*B15)</f>
+        <f t="shared" si="0"/>
         <v>5.8599999999999999E-2</v>
       </c>
       <c r="I15" s="5">
@@ -1823,7 +1823,7 @@
       <c r="B16" s="1">
         <v>1</v>
       </c>
-      <c r="C16" s="8" t="s">
+      <c r="C16" s="7" t="s">
         <v>43</v>
       </c>
       <c r="D16" s="1" t="s">
@@ -1839,7 +1839,7 @@
         <v>47</v>
       </c>
       <c r="H16" s="5">
-        <f>(I16*B16)</f>
+        <f t="shared" si="0"/>
         <v>1.03E-2</v>
       </c>
       <c r="I16" s="5">
@@ -1853,7 +1853,7 @@
       <c r="B17" s="1">
         <v>1</v>
       </c>
-      <c r="C17" s="8" t="s">
+      <c r="C17" s="7" t="s">
         <v>75</v>
       </c>
       <c r="D17" s="1" t="s">
@@ -1869,7 +1869,7 @@
         <v>76</v>
       </c>
       <c r="H17" s="5">
-        <f>(I17*B17)</f>
+        <f t="shared" si="0"/>
         <v>2.18E-2</v>
       </c>
       <c r="I17" s="5">
@@ -1883,7 +1883,7 @@
       <c r="B18" s="1">
         <v>7</v>
       </c>
-      <c r="C18" s="8" t="s">
+      <c r="C18" s="7" t="s">
         <v>61</v>
       </c>
       <c r="D18" s="1" t="s">
@@ -1899,7 +1899,7 @@
         <v>64</v>
       </c>
       <c r="H18" s="5">
-        <f>(I18*B18)</f>
+        <f t="shared" si="0"/>
         <v>8.3999999999999995E-3</v>
       </c>
       <c r="I18" s="5">
@@ -1913,7 +1913,7 @@
       <c r="B19" s="1">
         <v>1</v>
       </c>
-      <c r="C19" s="8" t="s">
+      <c r="C19" s="7" t="s">
         <v>65</v>
       </c>
       <c r="D19" s="1" t="s">
@@ -1929,7 +1929,7 @@
         <v>67</v>
       </c>
       <c r="H19" s="5">
-        <f>(I19*B19)</f>
+        <f t="shared" si="0"/>
         <v>1.2999999999999999E-3</v>
       </c>
       <c r="I19" s="5">
@@ -1943,7 +1943,7 @@
       <c r="B20" s="1">
         <v>3</v>
       </c>
-      <c r="C20" s="8" t="s">
+      <c r="C20" s="7" t="s">
         <v>68</v>
       </c>
       <c r="D20" s="1">
@@ -1959,7 +1959,7 @@
         <v>70</v>
       </c>
       <c r="H20" s="5">
-        <f>(I20*B20)</f>
+        <f t="shared" si="0"/>
         <v>3.0000000000000001E-3</v>
       </c>
       <c r="I20" s="5">
@@ -1973,7 +1973,7 @@
       <c r="B21" s="1">
         <v>2</v>
       </c>
-      <c r="C21" s="8" t="s">
+      <c r="C21" s="7" t="s">
         <v>118</v>
       </c>
       <c r="D21" s="1" t="s">
@@ -1989,7 +1989,7 @@
         <v>51</v>
       </c>
       <c r="H21" s="5">
-        <f>(I21*B21)</f>
+        <f t="shared" si="0"/>
         <v>4.48E-2</v>
       </c>
       <c r="I21" s="5">
@@ -2003,7 +2003,7 @@
       <c r="B22" s="1">
         <v>1</v>
       </c>
-      <c r="C22" s="8" t="s">
+      <c r="C22" s="7" t="s">
         <v>39</v>
       </c>
       <c r="D22" s="1" t="s">
@@ -2019,7 +2019,7 @@
         <v>40</v>
       </c>
       <c r="H22" s="5">
-        <f>(I22*B22)</f>
+        <f t="shared" si="0"/>
         <v>2.0472999999999999</v>
       </c>
       <c r="I22" s="5">
@@ -2033,7 +2033,7 @@
       <c r="B23" s="1">
         <v>1</v>
       </c>
-      <c r="C23" s="8" t="s">
+      <c r="C23" s="7" t="s">
         <v>9</v>
       </c>
       <c r="D23" s="1" t="s">
@@ -2049,7 +2049,7 @@
         <v>13</v>
       </c>
       <c r="H23" s="5">
-        <f>(I23*B23)</f>
+        <f t="shared" si="0"/>
         <v>6.5199999999999994E-2</v>
       </c>
       <c r="I23" s="5">
@@ -2063,7 +2063,7 @@
       <c r="B24" s="1">
         <v>1</v>
       </c>
-      <c r="C24" s="8" t="s">
+      <c r="C24" s="7" t="s">
         <v>14</v>
       </c>
       <c r="D24" s="1" t="s">
@@ -2079,7 +2079,7 @@
         <v>16</v>
       </c>
       <c r="H24" s="5">
-        <f>(I24*B24)</f>
+        <f t="shared" si="0"/>
         <v>0.06</v>
       </c>
       <c r="I24" s="5">
@@ -2093,7 +2093,7 @@
       <c r="B25" s="1">
         <v>1</v>
       </c>
-      <c r="C25" s="8" t="s">
+      <c r="C25" s="7" t="s">
         <v>26</v>
       </c>
       <c r="D25" s="1" t="s">
@@ -2109,7 +2109,7 @@
         <v>27</v>
       </c>
       <c r="H25" s="5">
-        <f>(I25*B25)</f>
+        <f t="shared" si="0"/>
         <v>0.28160000000000002</v>
       </c>
       <c r="I25" s="5">
@@ -2123,7 +2123,7 @@
       <c r="B26" s="1">
         <v>1</v>
       </c>
-      <c r="C26" s="8" t="s">
+      <c r="C26" s="7" t="s">
         <v>57</v>
       </c>
       <c r="D26" s="1" t="s">
@@ -2139,7 +2139,7 @@
         <v>60</v>
       </c>
       <c r="H26" s="5">
-        <f>(I26*B26)</f>
+        <f t="shared" si="0"/>
         <v>0.33250000000000002</v>
       </c>
       <c r="I26" s="5">
@@ -2157,7 +2157,7 @@
     <row r="29" spans="2:10" x14ac:dyDescent="0.4">
       <c r="H29" s="5">
         <f>SUM(H4:H26)</f>
-        <v>4.8148999999999997</v>
+        <v>4.8088999999999995</v>
       </c>
     </row>
   </sheetData>

</xml_diff>